<commit_message>
Adding worst fit algorithm and fixing bug in bandwidth calculation b/w switches
</commit_message>
<xml_diff>
--- a/vne/Results.xlsx
+++ b/vne/Results.xlsx
@@ -511,41 +511,41 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>random-testing-algorithm</t>
+          <t>worst-fit-algorithm</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>922</v>
+        <v>317</v>
       </c>
       <c r="D2" t="n">
-        <v>1607</v>
+        <v>664</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5737398879900436</v>
+        <v>0.4774096385542169</v>
       </c>
       <c r="F2" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G2" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H2" t="n">
-        <v>0.8571428571428571</v>
+        <v>0.3</v>
       </c>
       <c r="I2" t="n">
-        <v>4231</v>
+        <v>4250</v>
       </c>
       <c r="J2" t="n">
-        <v>2624</v>
+        <v>3586</v>
       </c>
       <c r="K2" t="n">
-        <v>1607</v>
+        <v>664</v>
       </c>
       <c r="L2" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="M2" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="N2" t="n">
         <v>18</v>

</xml_diff>

<commit_message>
Adding execution_time, num_vnrs_list support, and ignoring final layer of modified spine-leaf links
</commit_message>
<xml_diff>
--- a/vne/Results.xlsx
+++ b/vne/Results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P5"/>
+  <dimension ref="B1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,213 +509,10 @@
           <t>total_links</t>
         </is>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>7614</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>first-fit-algorithm</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>73</v>
-      </c>
-      <c r="E2" t="n">
-        <v>106</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.6886792452830188</v>
-      </c>
-      <c r="G2" t="n">
-        <v>2</v>
-      </c>
-      <c r="H2" t="n">
-        <v>2</v>
-      </c>
-      <c r="I2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" t="n">
-        <v>1178</v>
-      </c>
-      <c r="K2" t="n">
-        <v>1072</v>
-      </c>
-      <c r="L2" t="n">
-        <v>106</v>
-      </c>
-      <c r="M2" t="n">
-        <v>6</v>
-      </c>
-      <c r="N2" t="n">
-        <v>3</v>
-      </c>
-      <c r="O2" t="n">
-        <v>12</v>
-      </c>
-      <c r="P2" t="n">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>7614</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>worst-fit-algorithm</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>73</v>
-      </c>
-      <c r="E3" t="n">
-        <v>128</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.5703125</v>
-      </c>
-      <c r="G3" t="n">
-        <v>2</v>
-      </c>
-      <c r="H3" t="n">
-        <v>2</v>
-      </c>
-      <c r="I3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" t="n">
-        <v>1178</v>
-      </c>
-      <c r="K3" t="n">
-        <v>1050</v>
-      </c>
-      <c r="L3" t="n">
-        <v>128</v>
-      </c>
-      <c r="M3" t="n">
-        <v>11</v>
-      </c>
-      <c r="N3" t="n">
-        <v>4</v>
-      </c>
-      <c r="O3" t="n">
-        <v>12</v>
-      </c>
-      <c r="P3" t="n">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>1118</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>first-fit-algorithm</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>64</v>
-      </c>
-      <c r="E4" t="n">
-        <v>82</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.7804878048780488</v>
-      </c>
-      <c r="G4" t="n">
-        <v>2</v>
-      </c>
-      <c r="H4" t="n">
-        <v>2</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" t="n">
-        <v>1183</v>
-      </c>
-      <c r="K4" t="n">
-        <v>1101</v>
-      </c>
-      <c r="L4" t="n">
-        <v>82</v>
-      </c>
-      <c r="M4" t="n">
-        <v>4</v>
-      </c>
-      <c r="N4" t="n">
-        <v>2</v>
-      </c>
-      <c r="O4" t="n">
-        <v>12</v>
-      </c>
-      <c r="P4" t="n">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>1118</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>worst-fit-algorithm</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>64</v>
-      </c>
-      <c r="E5" t="n">
-        <v>94</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.6808510638297872</v>
-      </c>
-      <c r="G5" t="n">
-        <v>2</v>
-      </c>
-      <c r="H5" t="n">
-        <v>2</v>
-      </c>
-      <c r="I5" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" t="n">
-        <v>1183</v>
-      </c>
-      <c r="K5" t="n">
-        <v>1089</v>
-      </c>
-      <c r="L5" t="n">
-        <v>94</v>
-      </c>
-      <c r="M5" t="n">
-        <v>12</v>
-      </c>
-      <c r="N5" t="n">
-        <v>4</v>
-      </c>
-      <c r="O5" t="n">
-        <v>12</v>
-      </c>
-      <c r="P5" t="n">
-        <v>32</v>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>execution_time</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding output result attributes for avg link, crb, node utilizations
</commit_message>
<xml_diff>
--- a/vne/Results.xlsx
+++ b/vne/Results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,7 +511,27 @@
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>execution_time</t>
+          <t>total_execution_time</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>avg_bandwidth_utilization</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>avg_crb_utilization</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>avg_link_utilization</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>avg_node_utilization</t>
         </is>
       </c>
     </row>
@@ -520,7 +540,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>8734</v>
+        <v>5179</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -528,31 +548,31 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E2" t="n">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8653846153846154</v>
+        <v>0.8478260869565217</v>
       </c>
       <c r="G2" t="n">
         <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J2" t="n">
-        <v>1201</v>
+        <v>1191</v>
       </c>
       <c r="K2" t="n">
-        <v>1149</v>
+        <v>1145</v>
       </c>
       <c r="L2" t="n">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="M2" t="n">
         <v>3</v>
@@ -567,7 +587,19 @@
         <v>20</v>
       </c>
       <c r="Q2" t="n">
-        <v>45.3107533454895</v>
+        <v>48.32838821411133</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.4259740259740259</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.1515343915343915</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.25</v>
       </c>
     </row>
     <row r="3">
@@ -575,7 +607,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>8734</v>
+        <v>5179</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -583,37 +615,37 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="E3" t="n">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7758620689655172</v>
+        <v>0.7368421052631579</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3" t="n">
         <v>1</v>
       </c>
       <c r="J3" t="n">
-        <v>1201</v>
+        <v>1191</v>
       </c>
       <c r="K3" t="n">
-        <v>1143</v>
+        <v>1096</v>
       </c>
       <c r="L3" t="n">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="M3" t="n">
+        <v>8</v>
+      </c>
+      <c r="N3" t="n">
         <v>5</v>
-      </c>
-      <c r="N3" t="n">
-        <v>3</v>
       </c>
       <c r="O3" t="n">
         <v>12</v>
@@ -622,7 +654,19 @@
         <v>20</v>
       </c>
       <c r="Q3" t="n">
-        <v>45.49166107177734</v>
+        <v>62.37686014175415</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.2784735421779032</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.1555357624831309</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.4166666666666667</v>
       </c>
     </row>
     <row r="4">
@@ -630,7 +674,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>8734</v>
+        <v>7914</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -638,31 +682,31 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="E4" t="n">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8653846153846154</v>
+        <v>0.8734177215189873</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4" t="n">
         <v>2</v>
       </c>
       <c r="I4" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>1201</v>
+        <v>1107</v>
       </c>
       <c r="K4" t="n">
-        <v>1149</v>
+        <v>1028</v>
       </c>
       <c r="L4" t="n">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="M4" t="n">
         <v>3</v>
@@ -677,7 +721,19 @@
         <v>20</v>
       </c>
       <c r="Q4" t="n">
-        <v>46.46221327781677</v>
+        <v>61.71800255775452</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.4464285714285714</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.2971364221364221</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0.25</v>
       </c>
     </row>
     <row r="5">
@@ -685,7 +741,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>8734</v>
+        <v>7914</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -693,13 +749,13 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="E5" t="n">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F5" t="n">
-        <v>0.7549019607843137</v>
+        <v>0.696969696969697</v>
       </c>
       <c r="G5" t="n">
         <v>2</v>
@@ -711,13 +767,13 @@
         <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>1201</v>
+        <v>1107</v>
       </c>
       <c r="K5" t="n">
-        <v>1099</v>
+        <v>1008</v>
       </c>
       <c r="L5" t="n">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="M5" t="n">
         <v>9</v>
@@ -732,447 +788,19 @@
         <v>20</v>
       </c>
       <c r="Q5" t="n">
-        <v>59.82670259475708</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>8734</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>first-fit-algorithm</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>45</v>
-      </c>
-      <c r="E6" t="n">
-        <v>52</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.8653846153846154</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" t="n">
-        <v>3</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.3333333333333333</v>
-      </c>
-      <c r="J6" t="n">
-        <v>1201</v>
-      </c>
-      <c r="K6" t="n">
-        <v>1149</v>
-      </c>
-      <c r="L6" t="n">
-        <v>52</v>
-      </c>
-      <c r="M6" t="n">
-        <v>3</v>
-      </c>
-      <c r="N6" t="n">
-        <v>3</v>
-      </c>
-      <c r="O6" t="n">
-        <v>12</v>
-      </c>
-      <c r="P6" t="n">
-        <v>20</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>47.31556797027588</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>8734</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>worst-fit-algorithm</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>106</v>
-      </c>
-      <c r="E7" t="n">
-        <v>143</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.7412587412587412</v>
-      </c>
-      <c r="G7" t="n">
-        <v>3</v>
-      </c>
-      <c r="H7" t="n">
-        <v>3</v>
-      </c>
-      <c r="I7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" t="n">
-        <v>1201</v>
-      </c>
-      <c r="K7" t="n">
-        <v>1058</v>
-      </c>
-      <c r="L7" t="n">
-        <v>143</v>
-      </c>
-      <c r="M7" t="n">
-        <v>11</v>
-      </c>
-      <c r="N7" t="n">
-        <v>7</v>
-      </c>
-      <c r="O7" t="n">
-        <v>12</v>
-      </c>
-      <c r="P7" t="n">
-        <v>20</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>74.61014246940613</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>8188</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>first-fit-algorithm</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>32</v>
-      </c>
-      <c r="E8" t="n">
-        <v>35</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.9142857142857143</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" t="n">
-        <v>1</v>
-      </c>
-      <c r="J8" t="n">
-        <v>1124</v>
-      </c>
-      <c r="K8" t="n">
-        <v>1089</v>
-      </c>
-      <c r="L8" t="n">
-        <v>35</v>
-      </c>
-      <c r="M8" t="n">
-        <v>2</v>
-      </c>
-      <c r="N8" t="n">
-        <v>2</v>
-      </c>
-      <c r="O8" t="n">
-        <v>12</v>
-      </c>
-      <c r="P8" t="n">
-        <v>20</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>41.87593173980713</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>8188</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>worst-fit-algorithm</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>32</v>
-      </c>
-      <c r="E9" t="n">
-        <v>41</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.7804878048780488</v>
-      </c>
-      <c r="G9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I9" t="n">
-        <v>1</v>
-      </c>
-      <c r="J9" t="n">
-        <v>1124</v>
-      </c>
-      <c r="K9" t="n">
-        <v>1083</v>
-      </c>
-      <c r="L9" t="n">
-        <v>41</v>
-      </c>
-      <c r="M9" t="n">
-        <v>4</v>
-      </c>
-      <c r="N9" t="n">
-        <v>2</v>
-      </c>
-      <c r="O9" t="n">
-        <v>12</v>
-      </c>
-      <c r="P9" t="n">
-        <v>20</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>41.48594951629639</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>8188</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>first-fit-algorithm</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>73</v>
-      </c>
-      <c r="E10" t="n">
-        <v>83</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.8795180722891566</v>
-      </c>
-      <c r="G10" t="n">
-        <v>2</v>
-      </c>
-      <c r="H10" t="n">
-        <v>2</v>
-      </c>
-      <c r="I10" t="n">
-        <v>1</v>
-      </c>
-      <c r="J10" t="n">
-        <v>1124</v>
-      </c>
-      <c r="K10" t="n">
-        <v>1041</v>
-      </c>
-      <c r="L10" t="n">
-        <v>83</v>
-      </c>
-      <c r="M10" t="n">
-        <v>3</v>
-      </c>
-      <c r="N10" t="n">
-        <v>3</v>
-      </c>
-      <c r="O10" t="n">
-        <v>12</v>
-      </c>
-      <c r="P10" t="n">
-        <v>20</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>60.42582821846008</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>8188</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>worst-fit-algorithm</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>73</v>
-      </c>
-      <c r="E11" t="n">
-        <v>103</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.7087378640776699</v>
-      </c>
-      <c r="G11" t="n">
-        <v>2</v>
-      </c>
-      <c r="H11" t="n">
-        <v>2</v>
-      </c>
-      <c r="I11" t="n">
-        <v>1</v>
-      </c>
-      <c r="J11" t="n">
-        <v>1124</v>
-      </c>
-      <c r="K11" t="n">
-        <v>1021</v>
-      </c>
-      <c r="L11" t="n">
-        <v>103</v>
-      </c>
-      <c r="M11" t="n">
-        <v>10</v>
-      </c>
-      <c r="N11" t="n">
-        <v>5</v>
-      </c>
-      <c r="O11" t="n">
-        <v>12</v>
-      </c>
-      <c r="P11" t="n">
-        <v>20</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>60.05810904502869</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="n">
-        <v>8188</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>first-fit-algorithm</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>102</v>
-      </c>
-      <c r="E12" t="n">
-        <v>115</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.8869565217391304</v>
-      </c>
-      <c r="G12" t="n">
-        <v>3</v>
-      </c>
-      <c r="H12" t="n">
-        <v>3</v>
-      </c>
-      <c r="I12" t="n">
-        <v>1</v>
-      </c>
-      <c r="J12" t="n">
-        <v>1124</v>
-      </c>
-      <c r="K12" t="n">
-        <v>1009</v>
-      </c>
-      <c r="L12" t="n">
-        <v>115</v>
-      </c>
-      <c r="M12" t="n">
-        <v>3</v>
-      </c>
-      <c r="N12" t="n">
-        <v>3</v>
-      </c>
-      <c r="O12" t="n">
-        <v>12</v>
-      </c>
-      <c r="P12" t="n">
-        <v>20</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>74.22720861434937</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="n">
-        <v>8188</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>worst-fit-algorithm</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>102</v>
-      </c>
-      <c r="E13" t="n">
-        <v>141</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0.723404255319149</v>
-      </c>
-      <c r="G13" t="n">
-        <v>3</v>
-      </c>
-      <c r="H13" t="n">
-        <v>3</v>
-      </c>
-      <c r="I13" t="n">
-        <v>1</v>
-      </c>
-      <c r="J13" t="n">
-        <v>1124</v>
-      </c>
-      <c r="K13" t="n">
-        <v>983</v>
-      </c>
-      <c r="L13" t="n">
-        <v>141</v>
-      </c>
-      <c r="M13" t="n">
-        <v>11</v>
-      </c>
-      <c r="N13" t="n">
-        <v>6</v>
-      </c>
-      <c r="O13" t="n">
-        <v>12</v>
-      </c>
-      <c r="P13" t="n">
-        <v>20</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>72.36465406417847</v>
+        <v>61.50663352012634</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.2472876831892177</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.1688763681131551</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0.4166666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding support for NORD algorithm, & modifying existing code to rank VNRs and hosts, & reorganizing vne_algorithms module
</commit_message>
<xml_diff>
--- a/vne/Results.xlsx
+++ b/vne/Results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -540,7 +540,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>5179</v>
+        <v>81</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -548,37 +548,37 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="E2" t="n">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8478260869565217</v>
+        <v>0.7701149425287356</v>
       </c>
       <c r="G2" t="n">
         <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>1191</v>
+        <v>1143</v>
       </c>
       <c r="K2" t="n">
-        <v>1145</v>
+        <v>1056</v>
       </c>
       <c r="L2" t="n">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="M2" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O2" t="n">
         <v>12</v>
@@ -587,19 +587,19 @@
         <v>20</v>
       </c>
       <c r="Q2" t="n">
-        <v>48.32838821411133</v>
+        <v>49.34388446807861</v>
       </c>
       <c r="R2" t="n">
-        <v>0.4259740259740259</v>
+        <v>0.3690639998689534</v>
       </c>
       <c r="S2" t="n">
-        <v>0.1515343915343915</v>
+        <v>0.2017369417862839</v>
       </c>
       <c r="T2" t="n">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="U2" t="n">
-        <v>0.25</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="3">
@@ -607,7 +607,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>5179</v>
+        <v>81</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -615,37 +615,37 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E3" t="n">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7368421052631579</v>
+        <v>0.6504854368932039</v>
       </c>
       <c r="G3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3" t="n">
         <v>1</v>
       </c>
       <c r="J3" t="n">
-        <v>1191</v>
+        <v>1143</v>
       </c>
       <c r="K3" t="n">
-        <v>1096</v>
+        <v>1040</v>
       </c>
       <c r="L3" t="n">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="M3" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O3" t="n">
         <v>12</v>
@@ -654,19 +654,19 @@
         <v>20</v>
       </c>
       <c r="Q3" t="n">
-        <v>62.37686014175415</v>
+        <v>53.64048075675964</v>
       </c>
       <c r="R3" t="n">
-        <v>0.2784735421779032</v>
+        <v>0.357070501514946</v>
       </c>
       <c r="S3" t="n">
-        <v>0.1555357624831309</v>
+        <v>0.1867144540455617</v>
       </c>
       <c r="T3" t="n">
-        <v>0.4</v>
+        <v>0.45</v>
       </c>
       <c r="U3" t="n">
-        <v>0.4166666666666667</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="4">
@@ -674,45 +674,45 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>7914</v>
+        <v>81</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>first-fit-algorithm</t>
+          <t>nord-algorithm</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E4" t="n">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8734177215189873</v>
+        <v>0.6504854368932039</v>
       </c>
       <c r="G4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4" t="n">
         <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>1107</v>
+        <v>1143</v>
       </c>
       <c r="K4" t="n">
-        <v>1028</v>
+        <v>1040</v>
       </c>
       <c r="L4" t="n">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="M4" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="N4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O4" t="n">
         <v>12</v>
@@ -721,86 +721,19 @@
         <v>20</v>
       </c>
       <c r="Q4" t="n">
-        <v>61.71800255775452</v>
+        <v>52.26946973800659</v>
       </c>
       <c r="R4" t="n">
-        <v>0.4464285714285714</v>
+        <v>0.4158672015814873</v>
       </c>
       <c r="S4" t="n">
-        <v>0.2971364221364221</v>
+        <v>0.1872084415976796</v>
       </c>
       <c r="T4" t="n">
-        <v>0.15</v>
+        <v>0.35</v>
       </c>
       <c r="U4" t="n">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>7914</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>worst-fit-algorithm</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>69</v>
-      </c>
-      <c r="E5" t="n">
-        <v>99</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.696969696969697</v>
-      </c>
-      <c r="G5" t="n">
-        <v>2</v>
-      </c>
-      <c r="H5" t="n">
-        <v>2</v>
-      </c>
-      <c r="I5" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" t="n">
-        <v>1107</v>
-      </c>
-      <c r="K5" t="n">
-        <v>1008</v>
-      </c>
-      <c r="L5" t="n">
-        <v>99</v>
-      </c>
-      <c r="M5" t="n">
-        <v>9</v>
-      </c>
-      <c r="N5" t="n">
-        <v>5</v>
-      </c>
-      <c r="O5" t="n">
-        <v>12</v>
-      </c>
-      <c r="P5" t="n">
-        <v>20</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>61.50663352012634</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0.2472876831892177</v>
-      </c>
-      <c r="S5" t="n">
-        <v>0.1688763681131551</v>
-      </c>
-      <c r="T5" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="U5" t="n">
-        <v>0.4166666666666667</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding NRM and AHP vne algorithms integration
</commit_message>
<xml_diff>
--- a/vne/Results.xlsx
+++ b/vne/Results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -540,7 +540,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>81</v>
+        <v>1167</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -548,31 +548,31 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="E2" t="n">
-        <v>87</v>
+        <v>110</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7701149425287356</v>
+        <v>0.7909090909090909</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="J2" t="n">
-        <v>1143</v>
+        <v>1134</v>
       </c>
       <c r="K2" t="n">
-        <v>1056</v>
+        <v>1024</v>
       </c>
       <c r="L2" t="n">
-        <v>87</v>
+        <v>110</v>
       </c>
       <c r="M2" t="n">
         <v>6</v>
@@ -587,13 +587,13 @@
         <v>20</v>
       </c>
       <c r="Q2" t="n">
-        <v>49.34388446807861</v>
+        <v>66.71520590782166</v>
       </c>
       <c r="R2" t="n">
-        <v>0.3690639998689534</v>
+        <v>0.4597860372316894</v>
       </c>
       <c r="S2" t="n">
-        <v>0.2017369417862839</v>
+        <v>0.2534008537325048</v>
       </c>
       <c r="T2" t="n">
         <v>0.3</v>
@@ -607,7 +607,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>81</v>
+        <v>1167</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -615,37 +615,37 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>67</v>
+        <v>196</v>
       </c>
       <c r="E3" t="n">
-        <v>103</v>
+        <v>308</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6504854368932039</v>
+        <v>0.6363636363636364</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H3" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I3" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="J3" t="n">
-        <v>1143</v>
+        <v>1134</v>
       </c>
       <c r="K3" t="n">
-        <v>1040</v>
+        <v>826</v>
       </c>
       <c r="L3" t="n">
-        <v>103</v>
+        <v>308</v>
       </c>
       <c r="M3" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="N3" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="O3" t="n">
         <v>12</v>
@@ -654,19 +654,19 @@
         <v>20</v>
       </c>
       <c r="Q3" t="n">
-        <v>53.64048075675964</v>
+        <v>118.1071224212646</v>
       </c>
       <c r="R3" t="n">
-        <v>0.357070501514946</v>
+        <v>0.5838763181313047</v>
       </c>
       <c r="S3" t="n">
-        <v>0.1867144540455617</v>
+        <v>0.273170041544108</v>
       </c>
       <c r="T3" t="n">
-        <v>0.45</v>
+        <v>0.7</v>
       </c>
       <c r="U3" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="4">
@@ -674,7 +674,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>81</v>
+        <v>1167</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -682,58 +682,1197 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>67</v>
+        <v>264</v>
       </c>
       <c r="E4" t="n">
-        <v>103</v>
+        <v>390</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6504854368932039</v>
+        <v>0.676923076923077</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H4" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I4" t="n">
         <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>1143</v>
+        <v>1134</v>
       </c>
       <c r="K4" t="n">
-        <v>1040</v>
+        <v>744</v>
       </c>
       <c r="L4" t="n">
-        <v>103</v>
+        <v>390</v>
       </c>
       <c r="M4" t="n">
+        <v>17</v>
+      </c>
+      <c r="N4" t="n">
+        <v>11</v>
+      </c>
+      <c r="O4" t="n">
+        <v>12</v>
+      </c>
+      <c r="P4" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>146.0919725894928</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.5990333644542712</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.2917905638229925</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0.9166666666666666</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1167</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>nrm-algorithm</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>204</v>
+      </c>
+      <c r="E5" t="n">
+        <v>291</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.7010309278350515</v>
+      </c>
+      <c r="G5" t="n">
+        <v>4</v>
+      </c>
+      <c r="H5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1134</v>
+      </c>
+      <c r="K5" t="n">
+        <v>843</v>
+      </c>
+      <c r="L5" t="n">
+        <v>291</v>
+      </c>
+      <c r="M5" t="n">
+        <v>14</v>
+      </c>
+      <c r="N5" t="n">
+        <v>8</v>
+      </c>
+      <c r="O5" t="n">
+        <v>12</v>
+      </c>
+      <c r="P5" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>117.8740062713623</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.4974092361037834</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.2997010008377414</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1167</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>ahp-algorithm</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>136</v>
+      </c>
+      <c r="E6" t="n">
+        <v>211</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.6445497630331753</v>
+      </c>
+      <c r="G6" t="n">
+        <v>3</v>
+      </c>
+      <c r="H6" t="n">
+        <v>5</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1134</v>
+      </c>
+      <c r="K6" t="n">
+        <v>923</v>
+      </c>
+      <c r="L6" t="n">
+        <v>211</v>
+      </c>
+      <c r="M6" t="n">
+        <v>13</v>
+      </c>
+      <c r="N6" t="n">
         <v>7</v>
       </c>
-      <c r="N4" t="n">
+      <c r="O6" t="n">
+        <v>12</v>
+      </c>
+      <c r="P6" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>93.49396109580994</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.4003416017528975</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.2191942212130307</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0.5833333333333334</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1167</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>first-fit-algorithm</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>59</v>
+      </c>
+      <c r="E7" t="n">
+        <v>66</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.8939393939393939</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2</v>
+      </c>
+      <c r="H7" t="n">
+        <v>10</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1134</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1068</v>
+      </c>
+      <c r="L7" t="n">
+        <v>66</v>
+      </c>
+      <c r="M7" t="n">
+        <v>2</v>
+      </c>
+      <c r="N7" t="n">
+        <v>2</v>
+      </c>
+      <c r="O7" t="n">
+        <v>12</v>
+      </c>
+      <c r="P7" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>55.88456773757935</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.5444444444444444</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.3519634703196347</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0.1666666666666667</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1167</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>worst-fit-algorithm</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>277</v>
+      </c>
+      <c r="E8" t="n">
+        <v>407</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.6805896805896806</v>
+      </c>
+      <c r="G8" t="n">
+        <v>6</v>
+      </c>
+      <c r="H8" t="n">
+        <v>10</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1134</v>
+      </c>
+      <c r="K8" t="n">
+        <v>727</v>
+      </c>
+      <c r="L8" t="n">
+        <v>407</v>
+      </c>
+      <c r="M8" t="n">
+        <v>17</v>
+      </c>
+      <c r="N8" t="n">
+        <v>11</v>
+      </c>
+      <c r="O8" t="n">
+        <v>12</v>
+      </c>
+      <c r="P8" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>153.7660992145538</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.5989751604618866</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0.3051678769119821</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0.9166666666666666</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1167</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>nord-algorithm</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>345</v>
+      </c>
+      <c r="E9" t="n">
+        <v>467</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.7387580299785867</v>
+      </c>
+      <c r="G9" t="n">
+        <v>7</v>
+      </c>
+      <c r="H9" t="n">
+        <v>10</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1134</v>
+      </c>
+      <c r="K9" t="n">
+        <v>667</v>
+      </c>
+      <c r="L9" t="n">
+        <v>467</v>
+      </c>
+      <c r="M9" t="n">
+        <v>15</v>
+      </c>
+      <c r="N9" t="n">
+        <v>11</v>
+      </c>
+      <c r="O9" t="n">
+        <v>12</v>
+      </c>
+      <c r="P9" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>183.5495026111603</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.7672245555116272</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.3832400129613018</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0.9166666666666666</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1167</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>nrm-algorithm</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>345</v>
+      </c>
+      <c r="E10" t="n">
+        <v>481</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.7172557172557172</v>
+      </c>
+      <c r="G10" t="n">
+        <v>7</v>
+      </c>
+      <c r="H10" t="n">
+        <v>10</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1134</v>
+      </c>
+      <c r="K10" t="n">
+        <v>653</v>
+      </c>
+      <c r="L10" t="n">
+        <v>481</v>
+      </c>
+      <c r="M10" t="n">
+        <v>18</v>
+      </c>
+      <c r="N10" t="n">
+        <v>12</v>
+      </c>
+      <c r="O10" t="n">
+        <v>12</v>
+      </c>
+      <c r="P10" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>184.1256556510925</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0.6609714181007191</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.3571855997064296</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="U10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1167</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>ahp-algorithm</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>226</v>
+      </c>
+      <c r="E11" t="n">
+        <v>316</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.7151898734177216</v>
+      </c>
+      <c r="G11" t="n">
+        <v>5</v>
+      </c>
+      <c r="H11" t="n">
+        <v>10</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1134</v>
+      </c>
+      <c r="K11" t="n">
+        <v>818</v>
+      </c>
+      <c r="L11" t="n">
+        <v>316</v>
+      </c>
+      <c r="M11" t="n">
+        <v>15</v>
+      </c>
+      <c r="N11" t="n">
+        <v>9</v>
+      </c>
+      <c r="O11" t="n">
+        <v>12</v>
+      </c>
+      <c r="P11" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>116.0186278820038</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0.4691697496606033</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.3044198229448443</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>3691</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>first-fit-algorithm</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>67</v>
+      </c>
+      <c r="E12" t="n">
+        <v>77</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.8701298701298701</v>
+      </c>
+      <c r="G12" t="n">
+        <v>2</v>
+      </c>
+      <c r="H12" t="n">
+        <v>5</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J12" t="n">
+        <v>1132</v>
+      </c>
+      <c r="K12" t="n">
+        <v>1055</v>
+      </c>
+      <c r="L12" t="n">
+        <v>77</v>
+      </c>
+      <c r="M12" t="n">
+        <v>3</v>
+      </c>
+      <c r="N12" t="n">
+        <v>3</v>
+      </c>
+      <c r="O12" t="n">
+        <v>12</v>
+      </c>
+      <c r="P12" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>65.72345924377441</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.5961538461538461</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0.2797220481358094</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="U12" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>3691</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>worst-fit-algorithm</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>194</v>
+      </c>
+      <c r="E13" t="n">
+        <v>300</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.6466666666666666</v>
+      </c>
+      <c r="G13" t="n">
         <v>4</v>
       </c>
-      <c r="O4" t="n">
-        <v>12</v>
-      </c>
-      <c r="P4" t="n">
-        <v>20</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>52.26946973800659</v>
-      </c>
-      <c r="R4" t="n">
-        <v>0.4158672015814873</v>
-      </c>
-      <c r="S4" t="n">
-        <v>0.1872084415976796</v>
-      </c>
-      <c r="T4" t="n">
-        <v>0.35</v>
-      </c>
-      <c r="U4" t="n">
-        <v>0.3333333333333333</v>
+      <c r="H13" t="n">
+        <v>5</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1132</v>
+      </c>
+      <c r="K13" t="n">
+        <v>832</v>
+      </c>
+      <c r="L13" t="n">
+        <v>300</v>
+      </c>
+      <c r="M13" t="n">
+        <v>15</v>
+      </c>
+      <c r="N13" t="n">
+        <v>9</v>
+      </c>
+      <c r="O13" t="n">
+        <v>12</v>
+      </c>
+      <c r="P13" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>122.9830932617188</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0.588985207125558</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0.244152424403484</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="U13" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>3691</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>nord-algorithm</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>130</v>
+      </c>
+      <c r="E14" t="n">
+        <v>196</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.6632653061224489</v>
+      </c>
+      <c r="G14" t="n">
+        <v>3</v>
+      </c>
+      <c r="H14" t="n">
+        <v>5</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J14" t="n">
+        <v>1132</v>
+      </c>
+      <c r="K14" t="n">
+        <v>936</v>
+      </c>
+      <c r="L14" t="n">
+        <v>196</v>
+      </c>
+      <c r="M14" t="n">
+        <v>10</v>
+      </c>
+      <c r="N14" t="n">
+        <v>6</v>
+      </c>
+      <c r="O14" t="n">
+        <v>12</v>
+      </c>
+      <c r="P14" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>98.54456663131714</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0.5214710533131586</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0.2402455112586152</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="U14" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>3691</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>nrm-algorithm</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>130</v>
+      </c>
+      <c r="E15" t="n">
+        <v>194</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.6701030927835051</v>
+      </c>
+      <c r="G15" t="n">
+        <v>3</v>
+      </c>
+      <c r="H15" t="n">
+        <v>5</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="J15" t="n">
+        <v>1132</v>
+      </c>
+      <c r="K15" t="n">
+        <v>938</v>
+      </c>
+      <c r="L15" t="n">
+        <v>194</v>
+      </c>
+      <c r="M15" t="n">
+        <v>13</v>
+      </c>
+      <c r="N15" t="n">
+        <v>7</v>
+      </c>
+      <c r="O15" t="n">
+        <v>12</v>
+      </c>
+      <c r="P15" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>98.38719058036804</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0.3982841135472714</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0.2095811037225346</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="U15" t="n">
+        <v>0.5833333333333334</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>3691</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>ahp-algorithm</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>197</v>
+      </c>
+      <c r="E16" t="n">
+        <v>311</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.6334405144694534</v>
+      </c>
+      <c r="G16" t="n">
+        <v>4</v>
+      </c>
+      <c r="H16" t="n">
+        <v>5</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="J16" t="n">
+        <v>1132</v>
+      </c>
+      <c r="K16" t="n">
+        <v>821</v>
+      </c>
+      <c r="L16" t="n">
+        <v>311</v>
+      </c>
+      <c r="M16" t="n">
+        <v>15</v>
+      </c>
+      <c r="N16" t="n">
+        <v>9</v>
+      </c>
+      <c r="O16" t="n">
+        <v>12</v>
+      </c>
+      <c r="P16" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>122.702968120575</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0.599083154662102</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0.2497412386474395</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>3691</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>first-fit-algorithm</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>66</v>
+      </c>
+      <c r="E17" t="n">
+        <v>75</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="G17" t="n">
+        <v>2</v>
+      </c>
+      <c r="H17" t="n">
+        <v>10</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J17" t="n">
+        <v>1132</v>
+      </c>
+      <c r="K17" t="n">
+        <v>1057</v>
+      </c>
+      <c r="L17" t="n">
+        <v>75</v>
+      </c>
+      <c r="M17" t="n">
+        <v>3</v>
+      </c>
+      <c r="N17" t="n">
+        <v>3</v>
+      </c>
+      <c r="O17" t="n">
+        <v>12</v>
+      </c>
+      <c r="P17" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>66.62383151054382</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0.5371794871794872</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0.279789117216963</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>3691</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>worst-fit-algorithm</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>220</v>
+      </c>
+      <c r="E18" t="n">
+        <v>328</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.6707317073170732</v>
+      </c>
+      <c r="G18" t="n">
+        <v>5</v>
+      </c>
+      <c r="H18" t="n">
+        <v>10</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J18" t="n">
+        <v>1132</v>
+      </c>
+      <c r="K18" t="n">
+        <v>804</v>
+      </c>
+      <c r="L18" t="n">
+        <v>328</v>
+      </c>
+      <c r="M18" t="n">
+        <v>15</v>
+      </c>
+      <c r="N18" t="n">
+        <v>9</v>
+      </c>
+      <c r="O18" t="n">
+        <v>12</v>
+      </c>
+      <c r="P18" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>133.7557706832886</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0.5657462823076858</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0.2888671216018062</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="U18" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>3691</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>nord-algorithm</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>220</v>
+      </c>
+      <c r="E19" t="n">
+        <v>316</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.6962025316455697</v>
+      </c>
+      <c r="G19" t="n">
+        <v>5</v>
+      </c>
+      <c r="H19" t="n">
+        <v>10</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J19" t="n">
+        <v>1132</v>
+      </c>
+      <c r="K19" t="n">
+        <v>816</v>
+      </c>
+      <c r="L19" t="n">
+        <v>316</v>
+      </c>
+      <c r="M19" t="n">
+        <v>13</v>
+      </c>
+      <c r="N19" t="n">
+        <v>9</v>
+      </c>
+      <c r="O19" t="n">
+        <v>12</v>
+      </c>
+      <c r="P19" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>136.8531703948975</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0.5990116945582533</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0.2973956030169259</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="U19" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>3691</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>nrm-algorithm</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>220</v>
+      </c>
+      <c r="E20" t="n">
+        <v>300</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.7333333333333333</v>
+      </c>
+      <c r="G20" t="n">
+        <v>5</v>
+      </c>
+      <c r="H20" t="n">
+        <v>10</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J20" t="n">
+        <v>1132</v>
+      </c>
+      <c r="K20" t="n">
+        <v>832</v>
+      </c>
+      <c r="L20" t="n">
+        <v>300</v>
+      </c>
+      <c r="M20" t="n">
+        <v>15</v>
+      </c>
+      <c r="N20" t="n">
+        <v>11</v>
+      </c>
+      <c r="O20" t="n">
+        <v>12</v>
+      </c>
+      <c r="P20" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>135.5122628211975</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0.4949143643880486</v>
+      </c>
+      <c r="S20" t="n">
+        <v>0.2473751169973988</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="U20" t="n">
+        <v>0.9166666666666666</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>3691</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>ahp-algorithm</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>220</v>
+      </c>
+      <c r="E21" t="n">
+        <v>322</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.6832298136645962</v>
+      </c>
+      <c r="G21" t="n">
+        <v>5</v>
+      </c>
+      <c r="H21" t="n">
+        <v>10</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J21" t="n">
+        <v>1132</v>
+      </c>
+      <c r="K21" t="n">
+        <v>810</v>
+      </c>
+      <c r="L21" t="n">
+        <v>322</v>
+      </c>
+      <c r="M21" t="n">
+        <v>15</v>
+      </c>
+      <c r="N21" t="n">
+        <v>9</v>
+      </c>
+      <c r="O21" t="n">
+        <v>12</v>
+      </c>
+      <c r="P21" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>139.494934797287</v>
+      </c>
+      <c r="R21" t="n">
+        <v>0.5520662002065511</v>
+      </c>
+      <c r="S21" t="n">
+        <v>0.2889540630033016</v>
+      </c>
+      <c r="T21" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="U21" t="n">
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>